<commit_message>
added "Incident required" column
</commit_message>
<xml_diff>
--- a/external data sources/NASEM/nasem_instructions.xlsx
+++ b/external data sources/NASEM/nasem_instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medcornell-my.sharepoint.com/personal/saa3011_med_cornell_edu/Documents/Work/Mark Weiner/RECOVER/Queries/NASEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{5FB20629-5101-4695-878E-0A1ED0177F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FA40E3E-70D5-4FD0-9D34-5CF7A231A646}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{5FB20629-5101-4695-878E-0A1ED0177F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{408FB4B5-1D1A-4691-9208-A1D298FC840E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{20F07C32-D7F1-43DB-A2F9-257DDAA66EFE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
   <si>
     <t>NASEM principle</t>
   </si>
@@ -353,6 +353,15 @@
   </si>
   <si>
     <t>mood disorder</t>
+  </si>
+  <si>
+    <t>Incident required</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -571,10 +580,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1022,523 +1027,613 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="30.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7265625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.81640625" style="1"/>
+    <col min="2" max="3" width="20.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="30.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7265625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="1">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="1">
         <v>1</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="1">
         <v>1</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="1">
         <v>1</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:8" ht="14.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1546,6 +1641,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fca2c37e-528b-44ce-8718-33181a43e81d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6854e80a-0655-426b-88b1-65fb4535dc20" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B03BD8C70F62D448B4170DFC49C9C809" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a11703ed2302d032051714e2b6defb2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6854e80a-0655-426b-88b1-65fb4535dc20" xmlns:ns3="fca2c37e-528b-44ce-8718-33181a43e81d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="90954d470dc01e148744766dda6e1aac" ns2:_="" ns3:_="">
     <xsd:import namespace="6854e80a-0655-426b-88b1-65fb4535dc20"/>
@@ -1774,27 +1889,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fca2c37e-528b-44ce-8718-33181a43e81d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6854e80a-0655-426b-88b1-65fb4535dc20" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13482D1A-587C-489C-97FE-0D0C5722CBCC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fca2c37e-528b-44ce-8718-33181a43e81d"/>
+    <ds:schemaRef ds:uri="6854e80a-0655-426b-88b1-65fb4535dc20"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{261E3FAB-66A4-4FA7-A7AA-71E16895BDC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A24B38D8-3AA7-437B-A940-A2676FAAAB19}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1811,23 +1925,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13482D1A-587C-489C-97FE-0D0C5722CBCC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fca2c37e-528b-44ce-8718-33181a43e81d"/>
-    <ds:schemaRef ds:uri="6854e80a-0655-426b-88b1-65fb4535dc20"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{261E3FAB-66A4-4FA7-A7AA-71E16895BDC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>